<commit_message>
Modified adding items to service. If item has a bom, all bom items will be added to the service individually, if not selected item will be added.
</commit_message>
<xml_diff>
--- a/ServiceMaster/schedule/Need to be update.xlsx
+++ b/ServiceMaster/schedule/Need to be update.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="35">
   <si>
     <t>Add milage to vehicle service</t>
   </si>
@@ -97,6 +97,30 @@
   </si>
   <si>
     <t>Current date</t>
+  </si>
+  <si>
+    <t>Issue method to get from database</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Add employees to service</t>
+  </si>
+  <si>
+    <t>Modification</t>
+  </si>
+  <si>
+    <t>Remove service status from UI</t>
+  </si>
+  <si>
+    <t>.5 h</t>
+  </si>
+  <si>
+    <t>Activate manager functions with authorized user name password</t>
+  </si>
+  <si>
+    <t>Show reorder level reach with red color</t>
   </si>
 </sst>
 </file>
@@ -147,10 +171,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -556,20 +583,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:P5"/>
+  <dimension ref="B2:P10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" customWidth="1"/>
     <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="12.140625" bestFit="1" customWidth="1"/>
@@ -648,7 +675,7 @@
         <v>12</v>
       </c>
       <c r="J4" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="L4" t="s">
         <v>17</v>
@@ -674,7 +701,7 @@
         <v>24</v>
       </c>
       <c r="J5" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="L5" t="s">
         <v>17</v>
@@ -684,6 +711,136 @@
       </c>
       <c r="P5" s="1">
         <v>42947</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L6" t="s">
+        <v>17</v>
+      </c>
+      <c r="N6" s="1">
+        <v>42981</v>
+      </c>
+      <c r="P6" s="1">
+        <v>42980</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" t="s">
+        <v>24</v>
+      </c>
+      <c r="J7" t="s">
+        <v>13</v>
+      </c>
+      <c r="L7" t="s">
+        <v>15</v>
+      </c>
+      <c r="N7" s="1">
+        <v>42981</v>
+      </c>
+      <c r="P7" s="1">
+        <v>42980</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" t="s">
+        <v>32</v>
+      </c>
+      <c r="J8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L8" t="s">
+        <v>15</v>
+      </c>
+      <c r="N8" s="1">
+        <v>42981</v>
+      </c>
+      <c r="P8" s="1">
+        <v>42980</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" t="s">
+        <v>24</v>
+      </c>
+      <c r="J9" t="s">
+        <v>13</v>
+      </c>
+      <c r="L9" t="s">
+        <v>15</v>
+      </c>
+      <c r="N9" s="1">
+        <v>42983</v>
+      </c>
+      <c r="P9" s="1">
+        <v>42980</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J10" t="s">
+        <v>16</v>
+      </c>
+      <c r="L10" t="s">
+        <v>15</v>
+      </c>
+      <c r="N10" s="1">
+        <v>42983</v>
+      </c>
+      <c r="P10" s="1">
+        <v>42980</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added functionality to handle canceled item in services. Changed the invoice to handle this too.
</commit_message>
<xml_diff>
--- a/ServiceMaster/schedule/Need to be update.xlsx
+++ b/ServiceMaster/schedule/Need to be update.xlsx
@@ -586,7 +586,7 @@
   <dimension ref="B2:P10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -779,7 +779,7 @@
         <v>32</v>
       </c>
       <c r="J8" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="L8" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
Add functions and database tables to get issue method from database in item frame. Change all save functions to same format.
</commit_message>
<xml_diff>
--- a/ServiceMaster/schedule/Need to be update.xlsx
+++ b/ServiceMaster/schedule/Need to be update.xlsx
@@ -586,7 +586,7 @@
   <dimension ref="B2:P10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -727,7 +727,7 @@
         <v>24</v>
       </c>
       <c r="J6" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="L6" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
added database table for map services and employees. modified uom conversion table, corrected few GUI flows.
</commit_message>
<xml_diff>
--- a/ServiceMaster/schedule/Need to be update.xlsx
+++ b/ServiceMaster/schedule/Need to be update.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="36">
   <si>
     <t>Add milage to vehicle service</t>
   </si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t>Show reorder level reach with red color</t>
+  </si>
+  <si>
+    <t>Add view history for a vahicle in service form</t>
   </si>
 </sst>
 </file>
@@ -583,10 +586,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:P10"/>
+  <dimension ref="B2:P11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -755,9 +758,6 @@
       <c r="J7" t="s">
         <v>13</v>
       </c>
-      <c r="L7" t="s">
-        <v>15</v>
-      </c>
       <c r="N7" s="1">
         <v>42981</v>
       </c>
@@ -781,9 +781,6 @@
       <c r="J8" t="s">
         <v>28</v>
       </c>
-      <c r="L8" t="s">
-        <v>15</v>
-      </c>
       <c r="N8" s="1">
         <v>42981</v>
       </c>
@@ -807,9 +804,6 @@
       <c r="J9" t="s">
         <v>13</v>
       </c>
-      <c r="L9" t="s">
-        <v>15</v>
-      </c>
       <c r="N9" s="1">
         <v>42983</v>
       </c>
@@ -833,14 +827,34 @@
       <c r="J10" t="s">
         <v>16</v>
       </c>
-      <c r="L10" t="s">
-        <v>15</v>
-      </c>
       <c r="N10" s="1">
         <v>42983</v>
       </c>
       <c r="P10" s="1">
         <v>42980</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" t="s">
+        <v>24</v>
+      </c>
+      <c r="J11" t="s">
+        <v>13</v>
+      </c>
+      <c r="N11" s="1">
+        <v>42987</v>
+      </c>
+      <c r="P11" s="1">
+        <v>42982</v>
       </c>
     </row>
   </sheetData>

</xml_diff>